<commit_message>
add FIR calc Mathlab coefficient
</commit_message>
<xml_diff>
--- a/FIR/Clalc_taps/Calc_taps_hex.xlsx
+++ b/FIR/Clalc_taps/Calc_taps_hex.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>tap0</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>tap14</t>
+  </si>
+  <si>
+    <t>tap15</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5">
-        <v>-2.6499999999999999E-2</v>
+        <v>3.3E-3</v>
       </c>
       <c r="C1" s="1">
         <f>2^15</f>
@@ -475,19 +478,19 @@
       </c>
       <c r="D1" s="4">
         <f>B1*C1</f>
-        <v>-868.35199999999998</v>
+        <v>108.1344</v>
       </c>
       <c r="E1" s="7">
         <f>D1</f>
-        <v>-868.35199999999998</v>
+        <v>108.1344</v>
       </c>
       <c r="F1" s="7">
         <f>E1</f>
-        <v>-868.35199999999998</v>
+        <v>108.1344</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>DEC2HEX(F1)</f>
-        <v>FFFFFFFC9C</v>
+        <v>6C</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -495,27 +498,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <v>-1.3599999999999999E-2</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C15" si="0">2^15</f>
+        <f t="shared" ref="C2:C16" si="0">2^15</f>
         <v>32768</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D15" si="1">B2*C2</f>
-        <v>0</v>
+        <f t="shared" ref="D2:D16" si="1">B2*C2</f>
+        <v>-445.64479999999998</v>
       </c>
       <c r="E2" s="7">
-        <f t="shared" ref="E2:F15" si="2">D2</f>
-        <v>0</v>
+        <f t="shared" ref="E2:F16" si="2">D2</f>
+        <v>-445.64479999999998</v>
       </c>
       <c r="F2" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-445.64479999999998</v>
       </c>
       <c r="G2" s="2" t="str">
-        <f t="shared" ref="G2:G15" si="3">DEC2HEX(F2)</f>
-        <v>0</v>
+        <f t="shared" ref="G2:G16" si="3">DEC2HEX(F2)</f>
+        <v>FFFFFFFE43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -523,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <v>4.41E-2</v>
+        <v>-5.3E-3</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
@@ -531,19 +534,19 @@
       </c>
       <c r="D3" s="4">
         <f t="shared" si="1"/>
-        <v>1445.0688</v>
+        <v>-173.6704</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="2"/>
-        <v>1445.0688</v>
+        <v>-173.6704</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="2"/>
-        <v>1445.0688</v>
+        <v>-173.6704</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>5A5</v>
+        <v>FFFFFFFF53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -551,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>4.0800000000000003E-2</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
@@ -559,19 +562,19 @@
       </c>
       <c r="D4" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1336.9344000000001</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1336.9344000000001</v>
       </c>
       <c r="F4" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1336.9344000000001</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -579,7 +582,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>-9.3399999999999997E-2</v>
+        <v>-1.04E-2</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
@@ -587,19 +590,19 @@
       </c>
       <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>-3060.5311999999999</v>
+        <v>-340.78719999999998</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="2"/>
-        <v>-3060.5311999999999</v>
+        <v>-340.78719999999998</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="2"/>
-        <v>-3060.5311999999999</v>
+        <v>-340.78719999999998</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFF40C</v>
+        <v>FFFFFFFEAC</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -607,7 +610,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>0</v>
+        <v>-0.1022</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
@@ -615,19 +618,19 @@
       </c>
       <c r="D6" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3348.8896</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-3348.8896</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-3348.8896</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>FFFFFFF2EC</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -635,7 +638,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>0.31390000000000001</v>
+        <v>9.9199999999999997E-2</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
@@ -643,19 +646,19 @@
       </c>
       <c r="D7" s="4">
         <f t="shared" si="1"/>
-        <v>10285.8752</v>
+        <v>3250.5855999999999</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="2"/>
-        <v>10285.8752</v>
+        <v>3250.5855999999999</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="2"/>
-        <v>10285.8752</v>
+        <v>3250.5855999999999</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>282D</v>
+        <v>CB2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -663,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>0.5</v>
+        <v>0.4854</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
@@ -671,19 +674,19 @@
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>16384</v>
+        <v>15905.5872</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="2"/>
-        <v>16384</v>
+        <v>15905.5872</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="2"/>
-        <v>16384</v>
+        <v>15905.5872</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>3E21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -691,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5">
-        <v>0.31390000000000001</v>
+        <v>0.4854</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
@@ -699,19 +702,19 @@
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>10285.8752</v>
+        <v>15905.5872</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="2"/>
-        <v>10285.8752</v>
+        <v>15905.5872</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="2"/>
-        <v>10285.8752</v>
+        <v>15905.5872</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>282D</v>
+        <v>3E21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -719,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>0</v>
+        <v>9.9199999999999997E-2</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
@@ -727,19 +730,19 @@
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3250.5855999999999</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3250.5855999999999</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3250.5855999999999</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>CB2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -747,7 +750,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5">
-        <v>-9.3399999999999997E-2</v>
+        <v>-0.1022</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
@@ -755,19 +758,19 @@
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>-3060.5311999999999</v>
+        <v>-3348.8896</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="2"/>
-        <v>-3060.5311999999999</v>
+        <v>-3348.8896</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="2"/>
-        <v>-3060.5311999999999</v>
+        <v>-3348.8896</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFF40C</v>
+        <v>FFFFFFF2EC</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -775,7 +778,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>0</v>
+        <v>-1.04E-2</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
@@ -783,19 +786,19 @@
       </c>
       <c r="D12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-340.78719999999998</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-340.78719999999998</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-340.78719999999998</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>FFFFFFFEAC</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -803,7 +806,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5">
-        <v>4.41E-2</v>
+        <v>4.0800000000000003E-2</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
@@ -811,19 +814,19 @@
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>1445.0688</v>
+        <v>1336.9344000000001</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="2"/>
-        <v>1445.0688</v>
+        <v>1336.9344000000001</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="2"/>
-        <v>1445.0688</v>
+        <v>1336.9344000000001</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>5A5</v>
+        <v>538</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -831,7 +834,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5">
-        <v>0</v>
+        <v>-5.3E-3</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
@@ -839,19 +842,19 @@
       </c>
       <c r="D14" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-173.6704</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-173.6704</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-173.6704</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>FFFFFFFF53</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -859,7 +862,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5">
-        <v>-2.6499999999999999E-2</v>
+        <v>-1.3599999999999999E-2</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
@@ -867,19 +870,47 @@
       </c>
       <c r="D15" s="4">
         <f t="shared" si="1"/>
-        <v>-868.35199999999998</v>
+        <v>-445.64479999999998</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="2"/>
-        <v>-868.35199999999998</v>
+        <v>-445.64479999999998</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="2"/>
-        <v>-868.35199999999998</v>
+        <v>-445.64479999999998</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFFC9C</v>
+        <v>FFFFFFFE43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>3.3E-3</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>108.1344</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="2"/>
+        <v>108.1344</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="2"/>
+        <v>108.1344</v>
+      </c>
+      <c r="G16" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>6C</v>
       </c>
     </row>
   </sheetData>

</xml_diff>